<commit_message>
Buildings sector data updates
</commit_message>
<xml_diff>
--- a/InputData/bldgs/CL/Component Lifetime.xlsx
+++ b/InputData/bldgs/CL/Component Lifetime.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\CL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/TARGET_eps-us-3.2.1/InputData/bldgs/CL/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11533B43-7995-F646-B7E8-019616847B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="23955" windowHeight="11565"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="23960" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="7" r:id="rId1"/>
@@ -18,12 +19,23 @@
     <sheet name="other components" sheetId="6" r:id="rId4"/>
     <sheet name="CL" sheetId="8" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="102">
   <si>
     <t>Lifetime (years)</t>
   </si>
@@ -326,12 +338,15 @@
   </si>
   <si>
     <t>Building Component (years)</t>
+  </si>
+  <si>
+    <t>For Mexico we used US values, since the building components technology and materials are similar.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -544,6 +559,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -579,6 +611,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -754,23 +803,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="61.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="61.5" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -778,123 +829,128 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>99</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -902,18 +958,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="55.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>61</v>
       </c>
@@ -921,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -929,7 +985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -937,7 +993,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -945,7 +1001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -953,7 +1009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -961,7 +1017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -969,7 +1025,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -977,7 +1033,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -985,7 +1041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -993,7 +1049,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -1002,7 +1058,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>83</v>
       </c>
@@ -1010,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1018,7 +1074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1026,7 +1082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1034,7 +1090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1042,7 +1098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1050,7 +1106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>67</v>
       </c>
@@ -1058,7 +1114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +1123,7 @@
         <v>15.833333333333334</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>84</v>
       </c>
@@ -1075,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -1083,7 +1139,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1091,7 +1147,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -1099,7 +1155,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1107,7 +1163,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -1118,7 +1174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -1126,7 +1182,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -1134,7 +1190,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -1145,7 +1201,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -1153,7 +1209,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -1161,7 +1217,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -1169,7 +1225,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>11</v>
       </c>
@@ -1178,7 +1234,7 @@
         <v>51.81818181818182</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
@@ -1186,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1194,7 +1250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1202,7 +1258,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1210,7 +1266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1218,7 +1274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1226,7 +1282,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -1234,7 +1290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1242,7 +1298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -1250,7 +1306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1258,7 +1314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -1266,7 +1322,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -1274,7 +1330,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1282,7 +1338,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -1290,7 +1346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -1298,7 +1354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -1306,7 +1362,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>11</v>
       </c>
@@ -1321,28 +1377,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1356,7 +1412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1371,32 +1427,32 @@
         <v>9.1324200913242013</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -1407,24 +1463,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="33.5" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -1435,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>1000</v>
       </c>
@@ -1446,7 +1502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>1000</v>
       </c>
@@ -1457,7 +1513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1000</v>
       </c>
@@ -1468,7 +1524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1000</v>
       </c>
@@ -1479,7 +1535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>1000</v>
       </c>
@@ -1490,7 +1546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="12" t="s">
         <v>11</v>
@@ -1506,7 +1562,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1516,15 +1572,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -1538,7 +1594,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -1555,7 +1611,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -1572,7 +1628,7 @@
         <v>15.833333333333334</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1589,7 +1645,7 @@
         <v>51.81818181818182</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1606,7 +1662,7 @@
         <v>9.1324200913242013</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>94</v>
       </c>
@@ -1623,7 +1679,7 @@
         <v>13.533333333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>95</v>
       </c>

</xml_diff>